<commit_message>
Program Functional and Complete
Program works...anything extra is good.
</commit_message>
<xml_diff>
--- a/Task2.xlsx
+++ b/Task2.xlsx
@@ -436,7 +436,17 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>frank</t>
+          <t>Yu Qiao</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Luc Van Gool</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Lei Zhang</t>
         </is>
       </c>
     </row>
@@ -445,33 +455,41 @@
         <v>2022</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>bill</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
         <v>2023</v>
       </c>
+      <c r="B3" s="1" t="n">
+        <v>25</v>
+      </c>
       <c r="C3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="inlineStr">
-        <is>
-          <t>jill</t>
-        </is>
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
         <v>2024</v>
       </c>
+      <c r="B4" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>15</v>
+      </c>
       <c r="D4" s="1" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -480,6 +498,15 @@
           <t>Total</t>
         </is>
       </c>
+      <c r="B5" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>